<commit_message>
Completed all mandatory fields.
</commit_message>
<xml_diff>
--- a/ICAO/Activity/VocExcel ICAO Activity.xlsx
+++ b/ICAO/Activity/VocExcel ICAO Activity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://casaau-my.sharepoint.com/personal/michael_henry_casa_gov_au/Documents/Documents/2022/2022-03 - Sector Ontology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="168" documentId="13_ncr:1_{01388C4C-7024-4003-8532-420C54653B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A8D0D15-80AE-4F0F-B3C8-1CC8F8BBF642}"/>
+  <xr:revisionPtr revIDLastSave="198" documentId="13_ncr:1_{01388C4C-7024-4003-8532-420C54653B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B80ABA87-598A-4A96-A6E5-1F56765FFE33}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5445" windowWidth="29040" windowHeight="15840" tabRatio="497" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="5445" windowWidth="29040" windowHeight="15840" tabRatio="497" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="165">
   <si>
     <t>Surround Australia Pty Ltd</t>
   </si>
@@ -1493,6 +1493,45 @@
   <si>
     <t>https://casa-henrym.github.io/ICAO/Activity/#Commercial%20Air%20Transport%20services,https://casa-henrym.github.io/ICAO/Activity/#General%20aviation,https://casa-henrym.github.io/ICAO/Activity/#Airport%20services,https://casa-henrym.github.io/ICAO/Activity/#Air%20Navigation%20Services,https://casa-henrym.github.io/ICAO/Activity/#Civil%20aviation%20manufacturing,https://casa-henrym.github.io/ICAO/Activity/#Aviation%20Training,https://casa-henrym.github.io/ICAO/Activity/#Maintenance%20and%20overhaul,https://casa-henrym.github.io/ICAO/Activity/#Regulatory%20functions,https://casa-henrym.github.io/ICAO/Activity/#Other%20activities</t>
   </si>
+  <si>
+    <t>Non-ICAO: a service which provides a passenger with flexibility around the route they take and the time they travel.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The commercial operation or use of aircraft by companies for the carriage of passenger or goods as an aid to the conduct of their business and the availability of the aircraft for whole aircraft charter, flown by a professional pilot(s) employed to fly the aircraft. </t>
+  </si>
+  <si>
+    <t>Non-ICAO: the use of aircraft as part of the construction of buildings and other structures.</t>
+  </si>
+  <si>
+    <t>Non-ICAO: The taking of photographs from an aircraft.</t>
+  </si>
+  <si>
+    <t>Non-ICAO: Aerial survey is a method of collecting geomatics or other imagery by using airplanes, helicopters, UAVs, balloons or other aerial methods.</t>
+  </si>
+  <si>
+    <t>Non-ICAO: the use of aircraft to detect and track targets.</t>
+  </si>
+  <si>
+    <t>Non-ICAO: the search for and provision of aid to people who are in distress or imminent danger.</t>
+  </si>
+  <si>
+    <t>Non-ICAO: a form of marketing in which an aircraft is utilized to create or display a marketing message.</t>
+  </si>
+  <si>
+    <t>Non-ICAO: Services provided at an airport.</t>
+  </si>
+  <si>
+    <t>Non-ICAO: the manufacture of aircraft and related components.</t>
+  </si>
+  <si>
+    <t>Non-ICAO: Training of flight crew.</t>
+  </si>
+  <si>
+    <t>Non-ICAO: Defining and enforcing regulations for the safe conduct of flight.</t>
+  </si>
+  <si>
+    <t>Non-ICAO: Other activities.</t>
+  </si>
 </sst>
 </file>
 
@@ -2017,7 +2056,7 @@
   </sheetPr>
   <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3374,7 +3413,7 @@
   </sheetPr>
   <dimension ref="A1:Z1043"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A82" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A40" workbookViewId="0">
       <selection activeCell="B5" sqref="B5:I130"/>
     </sheetView>
   </sheetViews>
@@ -19082,8 +19121,8 @@
   <dimension ref="A1:AC1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A26" sqref="A26:A32"/>
+      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -19278,8 +19317,12 @@
       <c r="C7" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="D7" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>72</v>
+      </c>
       <c r="F7" s="11"/>
       <c r="G7" s="16" t="s">
         <v>145</v>
@@ -19297,8 +19340,12 @@
       <c r="C8" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="D8" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>72</v>
+      </c>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
@@ -19325,7 +19372,7 @@
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29" ht="84" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
         <v>83</v>
       </c>
@@ -19335,8 +19382,12 @@
       <c r="C10" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="D10" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>72</v>
+      </c>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
@@ -19352,8 +19403,12 @@
       <c r="C11" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
+      <c r="D11" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>72</v>
+      </c>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
@@ -19510,7 +19565,7 @@
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
         <v>101</v>
       </c>
@@ -19520,14 +19575,18 @@
       <c r="C19" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
+      <c r="D19" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>72</v>
+      </c>
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="s">
         <v>103</v>
       </c>
@@ -19537,14 +19596,18 @@
       <c r="C20" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
+      <c r="D20" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>72</v>
+      </c>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="16" t="s">
         <v>105</v>
       </c>
@@ -19554,14 +19617,18 @@
       <c r="C21" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
+      <c r="D21" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>72</v>
+      </c>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A22" s="16" t="s">
         <v>107</v>
       </c>
@@ -19571,14 +19638,18 @@
       <c r="C22" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
+      <c r="D22" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>72</v>
+      </c>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A23" s="16" t="s">
         <v>109</v>
       </c>
@@ -19588,14 +19659,18 @@
       <c r="C23" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
+      <c r="D23" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>72</v>
+      </c>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="s">
         <v>111</v>
       </c>
@@ -19605,8 +19680,12 @@
       <c r="C24" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
+      <c r="D24" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>72</v>
+      </c>
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
@@ -19643,8 +19722,12 @@
       <c r="C26" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
+      <c r="D26" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>72</v>
+      </c>
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
       <c r="H26" s="11"/>
@@ -19671,7 +19754,7 @@
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A28" s="16" t="s">
         <v>120</v>
       </c>
@@ -19681,8 +19764,12 @@
       <c r="C28" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
+      <c r="D28" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>72</v>
+      </c>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
       <c r="H28" s="11"/>
@@ -19698,8 +19785,12 @@
       <c r="C29" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
+      <c r="D29" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>72</v>
+      </c>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
       <c r="H29" s="11"/>
@@ -19726,7 +19817,7 @@
       <c r="H30" s="11"/>
       <c r="I30" s="11"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A31" s="16" t="s">
         <v>126</v>
       </c>
@@ -19736,8 +19827,12 @@
       <c r="C31" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
+      <c r="D31" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>72</v>
+      </c>
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
       <c r="H31" s="11"/>
@@ -19753,8 +19848,12 @@
       <c r="C32" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
+      <c r="D32" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>72</v>
+      </c>
       <c r="F32" s="11"/>
       <c r="G32" s="11"/>
       <c r="H32" s="11"/>

</xml_diff>

<commit_message>
Changed organisations to CASA to work with VocExcel
</commit_message>
<xml_diff>
--- a/ICAO/Activity/VocExcel ICAO Activity.xlsx
+++ b/ICAO/Activity/VocExcel ICAO Activity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://casaau-my.sharepoint.com/personal/michael_henry_casa_gov_au/Documents/Documents/2022/2022-03 - Sector Ontology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="198" documentId="13_ncr:1_{01388C4C-7024-4003-8532-420C54653B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B80ABA87-598A-4A96-A6E5-1F56765FFE33}"/>
+  <xr:revisionPtr revIDLastSave="206" documentId="13_ncr:1_{01388C4C-7024-4003-8532-420C54653B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EECB88EE-71D3-4FF0-8EC4-855987CF3119}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5445" windowWidth="29040" windowHeight="15840" tabRatio="497" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="5445" windowWidth="29040" windowHeight="15840" tabRatio="497" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="166">
   <si>
     <t>Surround Australia Pty Ltd</t>
   </si>
@@ -1532,6 +1532,9 @@
   <si>
     <t>Non-ICAO: Other activities.</t>
   </si>
+  <si>
+    <t>CASA</t>
+  </si>
 </sst>
 </file>
 
@@ -2056,7 +2059,7 @@
   </sheetPr>
   <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3413,7 +3416,7 @@
   </sheetPr>
   <dimension ref="A1:Z1043"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A40" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B5" sqref="B5:I130"/>
     </sheetView>
   </sheetViews>
@@ -15966,8 +15969,8 @@
   </sheetPr>
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -16062,7 +16065,7 @@
         <v>27</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>65</v>
+        <v>165</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>28</v>
@@ -16076,7 +16079,7 @@
         <v>30</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>65</v>
+        <v>165</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>28</v>
@@ -19121,7 +19124,7 @@
   <dimension ref="A1:AC1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>

</xml_diff>